<commit_message>
Removed api and web client projects
</commit_message>
<xml_diff>
--- a/Functional/InventoryEntities.xlsx
+++ b/Functional/InventoryEntities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="213">
   <si>
     <t>UserID</t>
   </si>
@@ -38,31 +38,16 @@
     <t>Key Field</t>
   </si>
   <si>
-    <t>Unique name for login</t>
-  </si>
-  <si>
     <t>Nvarchar(100)</t>
   </si>
   <si>
-    <t>Email ID</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Field</t>
   </si>
   <si>
     <t>Datetime</t>
   </si>
   <si>
-    <t>ForeignKey</t>
-  </si>
-  <si>
     <t>Nvarchar(50)</t>
-  </si>
-  <si>
-    <t>Answer to Secret Question</t>
   </si>
   <si>
     <t xml:space="preserve">Question </t>
@@ -444,9 +429,6 @@
     <t>ItemType</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>nvarchar(200)</t>
   </si>
   <si>
@@ -465,15 +447,6 @@
     <t>CategoryId</t>
   </si>
   <si>
-    <t>DefaultLocationId</t>
-  </si>
-  <si>
-    <t>DefaultSublocation</t>
-  </si>
-  <si>
-    <t>nvarchar(100)</t>
-  </si>
-  <si>
     <t>ReorderPoint</t>
   </si>
   <si>
@@ -534,18 +507,9 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
     <t>IsActive</t>
   </si>
   <si>
-    <t>PictureFileAttachmentId</t>
-  </si>
-  <si>
     <t>SoUomName</t>
   </si>
   <si>
@@ -567,9 +531,6 @@
     <t>PoUomRatio</t>
   </si>
   <si>
-    <t>TrackSerials</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -679,6 +640,27 @@
   </si>
   <si>
     <t>Water Proof</t>
+  </si>
+  <si>
+    <t>ImageId</t>
+  </si>
+  <si>
+    <t>SKUCode</t>
+  </si>
+  <si>
+    <t>ProductVariant</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductVariantId</t>
+  </si>
+  <si>
+    <t>uniqueidentifier</t>
+  </si>
+  <si>
+    <t>Property</t>
   </si>
 </sst>
 </file>
@@ -710,7 +692,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,6 +702,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -746,6 +734,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1049,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1066,123 +1055,123 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="G2" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="H2" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="I2" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="K2" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="E3" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G3" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="H3" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G4" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="H4" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="H5" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="H6" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="H7" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1194,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q126"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,60 +1204,63 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="1"/>
+      <c r="F1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="M1" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>212</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>2</v>
@@ -1280,29 +1272,29 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F3" t="str">
         <f>"public " &amp; C3 &amp; IF(D3="Y", "?","") &amp; " "  &amp;  A3 &amp; " {get; set;}"</f>
         <v>public Guid ProductId {get; set;}</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K3" t="s">
         <v>4</v>
@@ -1312,13 +1304,13 @@
         <v>public short UserStatusID {get; set;}</v>
       </c>
       <c r="M3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
         <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Q3" t="str">
         <f t="shared" ref="Q3:Q10" si="0">"public " &amp; O3 &amp; " "  &amp;  M3 &amp; " {get; set;}"</f>
@@ -1327,45 +1319,42 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F40" si="1">"public " &amp; C4 &amp; IF(D4="Y", "?","") &amp; " "  &amp;  A4 &amp; " {get; set;}"</f>
+        <f t="shared" ref="F4:F21" si="1">"public " &amp; C4 &amp; IF(D4="Y", "?","") &amp; " "  &amp;  A4 &amp; " {get; set;}"</f>
         <v>public int Version {get; set;}</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ref="L4:L5" si="2">"public " &amp; I4 &amp; " "  &amp;  G4 &amp; " {get; set;}"</f>
         <v>public string UserStatus {get; set;}</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="N4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="0"/>
@@ -1374,19 +1363,16 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1396,23 +1382,23 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="2"/>
         <v>public string Description {get; set;}</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
@@ -1421,32 +1407,29 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
-        <v>public string Name {get; set;}</v>
+        <v>public string ProductName {get; set;}</v>
       </c>
       <c r="M6" t="s">
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="O6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
@@ -1458,39 +1441,36 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
+        <v>131</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
         <v>public string Description {get; set;}</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="M7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="O7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="P7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="0"/>
@@ -1499,26 +1479,23 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
         <v>public string Remarks {get; set;}</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>2</v>
@@ -1529,13 +1506,13 @@
         <v>1</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
@@ -1544,32 +1521,29 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
-        <v>public string BarCode {get; set;}</v>
+        <v>public int CategoryId {get; set;}</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K9" t="s">
         <v>4</v>
@@ -1579,13 +1553,13 @@
         <v>public short AddressTypeID {get; set;}</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="0"/>
@@ -1594,45 +1568,42 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v>public int CategoryId {get; set;}</v>
+        <v>public decimal? ReorderPoint {get; set;}</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ref="L10:L11" si="3">"public " &amp; I10 &amp; " "  &amp;  G10 &amp; " {get; set;}"</f>
         <v>public string AddressType {get; set;}</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="0"/>
@@ -1641,29 +1612,29 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
-        <v>public int? DefaultLocationId {get; set;}</v>
+        <v>public decimal? ReorderQuantity {get; set;}</v>
       </c>
       <c r="G11" t="s">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="3"/>
@@ -1672,59 +1643,59 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
-        <v>public string DefaultSublocation {get; set;}</v>
+        <v>public string Uom {get; set;}</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? ReorderPoint {get; set;}</v>
+        <v>public int LastModifiedBy {get; set;}</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? ReorderQuantity {get; set;}</v>
+        <v>public DateTime LastModifiedOn {get; set;}</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1732,23 +1703,23 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
-        <v>public string Uom {get; set;}</v>
+        <v>public int? ImageId {get; set;}</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>2</v>
@@ -1760,36 +1731,36 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? MasterPackQty {get; set;}</v>
+        <v>public string SoUomName {get; set;}</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="M16" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" t="str">
@@ -1799,23 +1770,23 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? InnerPackQty {get; set;}</v>
+        <v>public decimal SoUomRatioStd {get; set;}</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>2</v>
@@ -1826,16 +1797,16 @@
         <v>1</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="4"/>
@@ -1844,29 +1815,29 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? CaseLength {get; set;}</v>
+        <v>public decimal SoUomRatio {get; set;}</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K18" t="s">
         <v>4</v>
@@ -1876,13 +1847,13 @@
         <v>public short CountryID {get; set;}</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" t="str">
@@ -1892,42 +1863,42 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? CaseWidth {get; set;}</v>
+        <v>public string PoUomName {get; set;}</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="5"/>
         <v>public string Country {get; set;}</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" t="str">
@@ -1937,42 +1908,42 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D20" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? CaseHeight {get; set;}</v>
+        <v>public decimal PoUomRatioStd {get; set;}</v>
       </c>
       <c r="G20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="5"/>
         <v>public string CountryCode {get; set;}</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" t="str">
@@ -1982,42 +1953,42 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? CaseWeight {get; set;}</v>
+        <v>public decimal PoUomRatio {get; set;}</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H21" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I21" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="5"/>
         <v>public string ISDCode {get; set;}</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" t="str">
@@ -2026,46 +1997,30 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B22" t="s">
-        <v>151</v>
-      </c>
-      <c r="C22" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal? ProductLength {get; set;}</v>
-      </c>
       <c r="G22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="5"/>
         <v>public short CurrencyID {get; set;}</v>
       </c>
       <c r="M22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N22" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="O22" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="4"/>
@@ -2073,33 +2028,17 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C23" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" t="s">
-        <v>137</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal? ProductWidth {get; set;}</v>
-      </c>
       <c r="M23" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="4"/>
@@ -2107,30 +2046,14 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" t="s">
-        <v>151</v>
-      </c>
-      <c r="C24" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" t="s">
-        <v>137</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal? ProductHeight {get; set;}</v>
-      </c>
       <c r="M24" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" t="str">
@@ -2138,471 +2061,522 @@
         <v>public DateTime CreatedOn {get; set;}</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>164</v>
-      </c>
-      <c r="B25" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" t="s">
-        <v>137</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal? ProductWeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>165</v>
-      </c>
-      <c r="B26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" t="s">
-        <v>137</v>
-      </c>
-      <c r="F26" t="str">
-        <f t="shared" si="1"/>
-        <v>public int? LastVendorId {get; set;}</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>166</v>
-      </c>
-      <c r="B27" t="s">
-        <v>167</v>
-      </c>
-      <c r="C27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D27" t="s">
-        <v>136</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="1"/>
-        <v>public bool IsSellable {get; set;}</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>168</v>
-      </c>
-      <c r="B28" t="s">
-        <v>167</v>
-      </c>
-      <c r="C28" t="s">
-        <v>187</v>
-      </c>
-      <c r="D28" t="s">
-        <v>136</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="1"/>
-        <v>public bool IsPurchaseable {get; set;}</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>184</v>
-      </c>
-      <c r="B29" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" t="s">
-        <v>136</v>
-      </c>
-      <c r="F29" t="str">
-        <f t="shared" si="1"/>
-        <v>public int LastModifiedBy {get; set;}</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" t="s">
-        <v>119</v>
-      </c>
-      <c r="D30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" si="1"/>
-        <v>public DateTime LastModifiedOn {get; set;}</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" t="str">
-        <f t="shared" si="1"/>
-        <v>public DateTime Timestamp {get; set;}</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>172</v>
-      </c>
-      <c r="B32" t="s">
-        <v>167</v>
-      </c>
-      <c r="C32" t="s">
-        <v>187</v>
-      </c>
-      <c r="D32" t="s">
-        <v>136</v>
-      </c>
-      <c r="F32" t="str">
-        <f t="shared" si="1"/>
-        <v>public bool IsActive {get; set;}</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" t="s">
-        <v>137</v>
-      </c>
-      <c r="F33" t="str">
-        <f t="shared" si="1"/>
-        <v>public int? PictureFileAttachmentId {get; set;}</v>
-      </c>
-    </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>174</v>
-      </c>
-      <c r="B34" t="s">
-        <v>154</v>
-      </c>
-      <c r="C34" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" t="s">
-        <v>136</v>
-      </c>
-      <c r="F34" t="str">
-        <f t="shared" si="1"/>
-        <v>public string SoUomName {get; set;}</v>
-      </c>
+      <c r="A34" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>175</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>131</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal SoUomRatioStd {get; set;}</v>
+        <f>"public " &amp; C35 &amp; IF(D35="Y", "?","") &amp; " "  &amp;  A35 &amp; " {get; set;}"</f>
+        <v>public Guid ProductVariantId {get; set;}</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal SoUomRatio {get; set;}</v>
+        <f>"public " &amp; C36 &amp; IF(D36="Y", "?","") &amp; " "  &amp;  A36 &amp; " {get; set;}"</f>
+        <v>public string BarCode {get; set;}</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
-        <v>public string PoUomName {get; set;}</v>
+        <f>"public " &amp; C37 &amp; IF(D37="Y", "?","") &amp; " "  &amp;  A37 &amp; " {get; set;}"</f>
+        <v>public decimal? MasterPackQty {get; set;}</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal PoUomRatioStd {get; set;}</v>
+        <f>"public " &amp; C38 &amp; IF(D38="Y", "?","") &amp; " "  &amp;  A38 &amp; " {get; set;}"</f>
+        <v>public decimal? InnerPackQty {get; set;}</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal PoUomRatio {get; set;}</v>
+        <f>"public " &amp; C39 &amp; IF(D39="Y", "?","") &amp; " "  &amp;  A39 &amp; " {get; set;}"</f>
+        <v>public decimal? CaseLength {get; set;}</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s">
-        <v>187</v>
+        <v>118</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="1"/>
-        <v>public bool TrackSerials {get; set;}</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+        <f>"public " &amp; C40 &amp; IF(D40="Y", "?","") &amp; " "  &amp;  A40 &amp; " {get; set;}"</f>
+        <v>public decimal? CaseWidth {get; set;}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" t="s">
+        <v>132</v>
+      </c>
+      <c r="F41" t="str">
+        <f>"public " &amp; C41 &amp; IF(D41="Y", "?","") &amp; " "  &amp;  A41 &amp; " {get; set;}"</f>
+        <v>public decimal? CaseHeight {get; set;}</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
+      </c>
+      <c r="F42" t="str">
+        <f>"public " &amp; C42 &amp; IF(D42="Y", "?","") &amp; " "  &amp;  A42 &amp; " {get; set;}"</f>
+        <v>public decimal? CaseWeight {get; set;}</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" t="str">
+        <f>"public " &amp; C43 &amp; IF(D43="Y", "?","") &amp; " "  &amp;  A43 &amp; " {get; set;}"</f>
+        <v>public decimal? ProductLength {get; set;}</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F44" t="str">
+        <f>"public " &amp; C44 &amp; IF(D44="Y", "?","") &amp; " "  &amp;  A44 &amp; " {get; set;}"</f>
+        <v>public decimal? ProductWidth {get; set;}</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" t="s">
+        <v>132</v>
+      </c>
+      <c r="F45" t="str">
+        <f>"public " &amp; C45 &amp; IF(D45="Y", "?","") &amp; " "  &amp;  A45 &amp; " {get; set;}"</f>
+        <v>public decimal? ProductHeight {get; set;}</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" t="s">
+        <v>132</v>
+      </c>
+      <c r="F46" t="str">
+        <f>"public " &amp; C46 &amp; IF(D46="Y", "?","") &amp; " "  &amp;  A46 &amp; " {get; set;}"</f>
+        <v>public decimal? ProductWeight {get; set;}</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" t="s">
         <v>85</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" t="s">
+        <v>132</v>
+      </c>
+      <c r="F47" t="str">
+        <f>"public " &amp; C47 &amp; IF(D47="Y", "?","") &amp; " "  &amp;  A47 &amp; " {get; set;}"</f>
+        <v>public int? LastVendorId {get; set;}</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" t="s">
+        <v>174</v>
+      </c>
+      <c r="D48" t="s">
+        <v>131</v>
+      </c>
+      <c r="F48" t="str">
+        <f>"public " &amp; C48 &amp; IF(D48="Y", "?","") &amp; " "  &amp;  A48 &amp; " {get; set;}"</f>
+        <v>public bool IsSellable {get; set;}</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>159</v>
+      </c>
+      <c r="B49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" t="s">
+        <v>131</v>
+      </c>
+      <c r="F49" t="str">
+        <f>"public " &amp; C49 &amp; IF(D49="Y", "?","") &amp; " "  &amp;  A49 &amp; " {get; set;}"</f>
+        <v>public bool IsPurchaseable {get; set;}</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" t="s">
+        <v>174</v>
+      </c>
+      <c r="D50" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" t="str">
+        <f>"public " &amp; C50 &amp; IF(D50="Y", "?","") &amp; " "  &amp;  A50 &amp; " {get; set;}"</f>
+        <v>public bool IsActive {get; set;}</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" t="s">
+        <v>132</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" ref="F51:F52" si="6">"public " &amp; C51 &amp; IF(D51="Y", "?","") &amp; " "  &amp;  A51 &amp; " {get; set;}"</f>
+        <v>public int? ImageId {get; set;}</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>207</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>131</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="6"/>
+        <v>public string SKUCode {get; set;}</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>113</v>
+      </c>
+      <c r="E73" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" ref="F73:F81" si="7">"public " &amp; C73 &amp; " "  &amp;  A73 &amp; " {get; set;}"</f>
+        <v>public Guid AddressID {get; set;}</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>113</v>
+      </c>
+      <c r="E74" t="s">
         <v>14</v>
       </c>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="F74" t="str">
+        <f t="shared" si="7"/>
+        <v>public Guid UserID {get; set;}</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" t="s">
+        <v>115</v>
+      </c>
+      <c r="E75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="7"/>
+        <v>public short AddressType {get; set;}</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>116</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="7"/>
+        <v>public string AddressLine1 {get; set;}</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" t="s">
+        <v>116</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="7"/>
+        <v>public string AddressLine2 {get; set;}</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>18</v>
       </c>
-      <c r="B91" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91" t="s">
-        <v>118</v>
-      </c>
-      <c r="E91" t="s">
-        <v>4</v>
-      </c>
-      <c r="F91" t="str">
-        <f t="shared" ref="F91:F99" si="6">"public " &amp; C91 &amp; " "  &amp;  A91 &amp; " {get; set;}"</f>
-        <v>public Guid AddressID {get; set;}</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92" t="s">
-        <v>118</v>
-      </c>
-      <c r="E92" t="s">
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>116</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="7"/>
+        <v>public string City {get; set;}</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>19</v>
       </c>
-      <c r="F92" t="str">
-        <f t="shared" si="6"/>
-        <v>public Guid UserID {get; set;}</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="B79" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" t="s">
+        <v>116</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="7"/>
+        <v>public string PostCode {get; set;}</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>20</v>
       </c>
-      <c r="B93" t="s">
-        <v>17</v>
-      </c>
-      <c r="C93" t="s">
-        <v>120</v>
-      </c>
-      <c r="E93" t="s">
-        <v>19</v>
-      </c>
-      <c r="F93" t="str">
-        <f t="shared" si="6"/>
-        <v>public short AddressType {get; set;}</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>21</v>
-      </c>
-      <c r="B94" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" t="s">
-        <v>121</v>
-      </c>
-      <c r="F94" t="str">
-        <f t="shared" si="6"/>
-        <v>public string AddressLine1 {get; set;}</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>116</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="7"/>
+        <v>public string State {get; set;}</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>22</v>
       </c>
-      <c r="B95" t="s">
-        <v>6</v>
-      </c>
-      <c r="C95" t="s">
-        <v>121</v>
-      </c>
-      <c r="F95" t="str">
-        <f t="shared" si="6"/>
-        <v>public string AddressLine2 {get; set;}</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>23</v>
-      </c>
-      <c r="B96" t="s">
-        <v>12</v>
-      </c>
-      <c r="C96" t="s">
-        <v>121</v>
-      </c>
-      <c r="F96" t="str">
-        <f t="shared" si="6"/>
-        <v>public string City {get; set;}</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="B81" t="s">
         <v>24</v>
       </c>
-      <c r="B97" t="s">
-        <v>28</v>
-      </c>
-      <c r="C97" t="s">
-        <v>121</v>
-      </c>
-      <c r="F97" t="str">
-        <f t="shared" si="6"/>
-        <v>public string PostCode {get; set;}</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>25</v>
-      </c>
-      <c r="B98" t="s">
-        <v>12</v>
-      </c>
-      <c r="C98" t="s">
-        <v>121</v>
-      </c>
-      <c r="F98" t="str">
-        <f t="shared" si="6"/>
-        <v>public string State {get; set;}</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>27</v>
-      </c>
-      <c r="B99" t="s">
-        <v>29</v>
-      </c>
-      <c r="C99" t="s">
-        <v>120</v>
-      </c>
-      <c r="E99" t="s">
-        <v>19</v>
-      </c>
-      <c r="F99" t="str">
-        <f t="shared" si="6"/>
+      <c r="C81" t="s">
+        <v>115</v>
+      </c>
+      <c r="E81" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="7"/>
         <v>public short CountryID {get; set;}</v>
       </c>
+    </row>
+    <row r="99" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:17" x14ac:dyDescent="0.25">
       <c r="M100" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="N100" s="4"/>
       <c r="O100" s="4"/>
       <c r="P100" s="4"/>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G101" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
       <c r="M101" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N101" s="1" t="s">
         <v>2</v>
@@ -2612,119 +2586,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H102" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I102" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K102" t="s">
         <v>4</v>
       </c>
       <c r="L102" t="str">
-        <f t="shared" ref="L102:L105" si="7">"public " &amp; I102 &amp; " "  &amp;  G102 &amp; " {get; set;}"</f>
+        <f t="shared" ref="L102:L105" si="8">"public " &amp; I102 &amp; " "  &amp;  G102 &amp; " {get; set;}"</f>
         <v>public short CurrencyID {get; set;}</v>
       </c>
       <c r="M102" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="N102" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O102" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q102" t="str">
-        <f t="shared" ref="Q102:Q126" si="8">"public " &amp; O102 &amp; " "  &amp;  M102 &amp; " {get; set;}"</f>
+        <f t="shared" ref="Q102:Q126" si="9">"public " &amp; O102 &amp; " "  &amp;  M102 &amp; " {get; set;}"</f>
         <v>public short VoucherTypeID {get; set;}</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G103" t="s">
+        <v>30</v>
+      </c>
+      <c r="H103" t="s">
+        <v>34</v>
+      </c>
+      <c r="I103" t="s">
+        <v>116</v>
+      </c>
+      <c r="L103" t="str">
+        <f t="shared" si="8"/>
+        <v>public string CurrencyCode {get; set;}</v>
+      </c>
+      <c r="M103" t="s">
+        <v>60</v>
+      </c>
+      <c r="N103" t="s">
+        <v>62</v>
+      </c>
+      <c r="O103" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q103" t="str">
+        <f t="shared" si="9"/>
+        <v>public string VoucherType {get; set;}</v>
+      </c>
+    </row>
+    <row r="104" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>33</v>
+      </c>
+      <c r="H104" t="s">
         <v>35</v>
       </c>
-      <c r="H103" t="s">
-        <v>39</v>
-      </c>
-      <c r="I103" t="s">
-        <v>121</v>
-      </c>
-      <c r="L103" t="str">
-        <f t="shared" si="7"/>
-        <v>public string CurrencyCode {get; set;}</v>
-      </c>
-      <c r="M103" t="s">
-        <v>65</v>
-      </c>
-      <c r="N103" t="s">
-        <v>67</v>
-      </c>
-      <c r="O103" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q103" t="str">
+      <c r="I104" t="s">
+        <v>116</v>
+      </c>
+      <c r="L104" t="str">
         <f t="shared" si="8"/>
-        <v>public string VoucherType {get; set;}</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G104" t="s">
-        <v>38</v>
-      </c>
-      <c r="H104" t="s">
-        <v>40</v>
-      </c>
-      <c r="I104" t="s">
-        <v>121</v>
-      </c>
-      <c r="L104" t="str">
-        <f t="shared" si="7"/>
         <v>public string CurrencySymbol {get; set;}</v>
       </c>
       <c r="M104" t="s">
         <v>1</v>
       </c>
       <c r="N104" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="O104" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q104" t="str">
+        <f t="shared" si="9"/>
+        <v>public string Description {get; set;}</v>
+      </c>
+    </row>
+    <row r="105" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>31</v>
+      </c>
+      <c r="H105" t="s">
+        <v>25</v>
+      </c>
+      <c r="I105" t="s">
+        <v>116</v>
+      </c>
+      <c r="L105" t="str">
         <f t="shared" si="8"/>
-        <v>public string Description {get; set;}</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G105" t="s">
-        <v>36</v>
-      </c>
-      <c r="H105" t="s">
-        <v>30</v>
-      </c>
-      <c r="I105" t="s">
-        <v>121</v>
-      </c>
-      <c r="L105" t="str">
-        <f t="shared" si="7"/>
         <v>public string Currency {get; set;}</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:17" x14ac:dyDescent="0.25">
       <c r="M107" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N107" s="4"/>
       <c r="O107" s="4"/>
       <c r="P107" s="4"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:17" x14ac:dyDescent="0.25">
       <c r="M108" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N108" s="1" t="s">
         <v>2</v>
@@ -2734,31 +2708,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G109" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
       <c r="M109" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="N109" t="s">
         <v>3</v>
       </c>
       <c r="O109" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Q109" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public Guid AccountID {get; set;}</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G110" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>2</v>
@@ -2775,46 +2749,46 @@
         <v>3</v>
       </c>
       <c r="O110" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="P110" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="Q110" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public Guid UserID {get; set;}</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="7:17" x14ac:dyDescent="0.25">
       <c r="M111" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N111" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O111" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="P111" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Q111" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public string Account {get; set;}</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="7:17" x14ac:dyDescent="0.25">
       <c r="M112" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N112" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O112" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q112" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public string CrDr {get; set;}</v>
       </c>
     </row>
@@ -2823,195 +2797,190 @@
         <v>1</v>
       </c>
       <c r="N113" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="O113" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q113" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public string Description {get; set;}</v>
       </c>
     </row>
     <row r="114" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M114" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="N114" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O114" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q114" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public short ParentAccountID {get; set;}</v>
       </c>
     </row>
     <row r="117" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M117" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N117" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O117" s="4"/>
       <c r="P117" s="4"/>
     </row>
     <row r="118" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M118" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N118" t="s">
         <v>3</v>
       </c>
       <c r="O118" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="P118" t="s">
         <v>4</v>
       </c>
       <c r="Q118" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public Guid AccountAddressID {get; set;}</v>
       </c>
     </row>
     <row r="119" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M119" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="N119" t="s">
         <v>3</v>
       </c>
       <c r="O119" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="P119" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="Q119" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public Guid AccountID {get; set;}</v>
       </c>
     </row>
     <row r="120" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M120" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N120" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="O120" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="P120" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="Q120" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public short AddressType {get; set;}</v>
       </c>
     </row>
     <row r="121" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M121" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="N121" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O121" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q121" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public string AddressLine1 {get; set;}</v>
       </c>
     </row>
     <row r="122" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M122" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="N122" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O122" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q122" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public string AddressLine2 {get; set;}</v>
       </c>
     </row>
     <row r="123" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M123" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N123" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O123" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q123" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public string City {get; set;}</v>
       </c>
     </row>
     <row r="124" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M124" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N124" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O124" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q124" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public string PostCode {get; set;}</v>
       </c>
     </row>
     <row r="125" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M125" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N125" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O125" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q125" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public string State {get; set;}</v>
       </c>
     </row>
     <row r="126" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M126" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="N126" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O126" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="P126" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="Q126" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>public short CountryID {get; set;}</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G16:K16"/>
+  <mergeCells count="13">
     <mergeCell ref="M117:P117"/>
     <mergeCell ref="G109:K109"/>
     <mergeCell ref="M1:P1"/>
@@ -3019,6 +2988,12 @@
     <mergeCell ref="M100:P100"/>
     <mergeCell ref="M107:P107"/>
     <mergeCell ref="G101:K101"/>
+    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3041,33 +3016,33 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3103,57 +3078,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3178,35 +3153,35 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3229,7 +3204,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B1">
         <v>2010</v>
@@ -3237,7 +3212,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -3245,7 +3220,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3253,73 +3228,73 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3344,48 +3319,48 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="105" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domain and Database projects are added
</commit_message>
<xml_diff>
--- a/Functional/InventoryEntities.xlsx
+++ b/Functional/InventoryEntities.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="228">
   <si>
     <t>UserID</t>
   </si>
@@ -423,9 +423,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>ItemType</t>
   </si>
   <si>
@@ -444,9 +441,6 @@
     <t>nvarchar(500)</t>
   </si>
   <si>
-    <t>CategoryId</t>
-  </si>
-  <si>
     <t>ReorderPoint</t>
   </si>
   <si>
@@ -456,12 +450,6 @@
     <t>ReorderQuantity</t>
   </si>
   <si>
-    <t>Uom</t>
-  </si>
-  <si>
-    <t>nvarchar(20)</t>
-  </si>
-  <si>
     <t>MasterPackQty</t>
   </si>
   <si>
@@ -510,27 +498,6 @@
     <t>IsActive</t>
   </si>
   <si>
-    <t>SoUomName</t>
-  </si>
-  <si>
-    <t>SoUomRatioStd</t>
-  </si>
-  <si>
-    <t>decimal(10, 4)</t>
-  </si>
-  <si>
-    <t>SoUomRatio</t>
-  </si>
-  <si>
-    <t>PoUomName</t>
-  </si>
-  <si>
-    <t>PoUomRatioStd</t>
-  </si>
-  <si>
-    <t>PoUomRatio</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -661,6 +628,84 @@
   </si>
   <si>
     <t>Property</t>
+  </si>
+  <si>
+    <t>SubCategoryId</t>
+  </si>
+  <si>
+    <t>SalesOrderUnitId</t>
+  </si>
+  <si>
+    <t>UnitId</t>
+  </si>
+  <si>
+    <t>PurchaseOrderUnitId</t>
+  </si>
+  <si>
+    <t>ProductImage</t>
+  </si>
+  <si>
+    <t>Uniqueidentifier</t>
+  </si>
+  <si>
+    <t>decimal(10, 2)</t>
+  </si>
+  <si>
+    <t>LastPurchasePrice</t>
+  </si>
+  <si>
+    <t>ShelfPrice</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>PromotionId</t>
+  </si>
+  <si>
+    <t>BasePrice</t>
+  </si>
+  <si>
+    <t>PromotionName</t>
+  </si>
+  <si>
+    <t>PromotionTypeId</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>PromotionText</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t>PromotionRule</t>
+  </si>
+  <si>
+    <t>AgentId</t>
+  </si>
+  <si>
+    <t>AgentProductVaiantPrice</t>
+  </si>
+  <si>
+    <t>PricingType</t>
+  </si>
+  <si>
+    <t>Flat / Percent</t>
+  </si>
+  <si>
+    <t>PricingValue</t>
+  </si>
+  <si>
+    <t>AgentProductVariantPriceId</t>
+  </si>
+  <si>
+    <t>UniquIdentifier</t>
   </si>
 </sst>
 </file>
@@ -731,10 +776,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,123 +1100,123 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="G2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="H2" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="I2" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="K2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="G3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="H3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H4" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H5" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H6" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H7" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1181,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q126"/>
+  <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,46 +1248,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="M1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>212</v>
+      <c r="F2" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -1272,10 +1317,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>113</v>
@@ -1331,8 +1376,8 @@
         <v>131</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F21" si="1">"public " &amp; C4 &amp; IF(D4="Y", "?","") &amp; " "  &amp;  A4 &amp; " {get; set;}"</f>
-        <v>public int Version {get; set;}</v>
+        <f t="shared" ref="F4:F16" si="1">"public " &amp; C4 &amp; IF(D4="Y", "?","") &amp; " "  &amp;  A4 &amp; " {get; set;}"</f>
+        <v>public int ItemType {get; set;}</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -1363,20 +1408,20 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
         <v>134</v>
       </c>
-      <c r="B5" t="s">
-        <v>85</v>
-      </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
         <v>131</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
-        <v>public int ItemType {get; set;}</v>
+        <v>public string ProductName {get; set;}</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
@@ -1407,7 +1452,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>135</v>
@@ -1420,7 +1465,7 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
-        <v>public string ProductName {get; set;}</v>
+        <v>public string Description {get; set;}</v>
       </c>
       <c r="M6" t="s">
         <v>1</v>
@@ -1438,10 +1483,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>116</v>
@@ -1451,15 +1496,15 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
-        <v>public string Description {get; set;}</v>
-      </c>
-      <c r="G7" s="4" t="s">
+        <v>public string Remarks {get; set;}</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
       <c r="M7" t="s">
         <v>41</v>
       </c>
@@ -1479,20 +1524,20 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>202</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D8" t="s">
         <v>131</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
-        <v>public string Remarks {get; set;}</v>
+        <v>public Guid SubCategoryId {get; set;}</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>6</v>
@@ -1521,20 +1566,20 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
         <v>140</v>
       </c>
-      <c r="B9" t="s">
-        <v>85</v>
-      </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
-        <v>public int CategoryId {get; set;}</v>
+        <v>public decimal? ReorderPoint {get; set;}</v>
       </c>
       <c r="G9" t="s">
         <v>26</v>
@@ -1571,7 +1616,7 @@
         <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
         <v>118</v>
@@ -1581,7 +1626,7 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? ReorderPoint {get; set;}</v>
+        <v>public decimal? ReorderQuantity {get; set;}</v>
       </c>
       <c r="G10" t="s">
         <v>15</v>
@@ -1612,20 +1657,20 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
-        <v>public decimal? ReorderQuantity {get; set;}</v>
+        <v>public Guid UnitId {get; set;}</v>
       </c>
       <c r="G11" t="s">
         <v>1</v>
@@ -1643,80 +1688,80 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
         <v>131</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
-        <v>public string Uom {get; set;}</v>
+        <v>public int LastModifiedBy {get; set;}</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
         <v>131</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
-        <v>public int LastModifiedBy {get; set;}</v>
+        <v>public DateTime LastModifiedOn {get; set;}</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
-        <v>public DateTime LastModifiedOn {get; set;}</v>
-      </c>
-      <c r="M14" s="4" t="s">
+        <v>public Guid? ImageId {get; set;}</v>
+      </c>
+      <c r="M14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>162</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
-        <v>public int? ImageId {get; set;}</v>
+        <v>public Guid SalesOrderUnitId {get; set;}</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>6</v>
@@ -1731,28 +1776,28 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" t="s">
         <v>162</v>
       </c>
-      <c r="B16" t="s">
-        <v>145</v>
-      </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
         <v>131</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
-        <v>public string SoUomName {get; set;}</v>
-      </c>
-      <c r="G16" s="4" t="s">
+        <v>public Guid PurchaseOrderUnitId {get; set;}</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
       <c r="M16" s="2" t="s">
         <v>47</v>
       </c>
@@ -1769,22 +1814,6 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" t="s">
-        <v>131</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal SoUomRatioStd {get; set;}</v>
-      </c>
       <c r="G17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1814,22 +1843,6 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>165</v>
-      </c>
-      <c r="B18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal SoUomRatio {get; set;}</v>
-      </c>
       <c r="G18" t="s">
         <v>22</v>
       </c>
@@ -1862,22 +1875,6 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C19" t="s">
-        <v>116</v>
-      </c>
-      <c r="D19" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="1"/>
-        <v>public string PoUomName {get; set;}</v>
-      </c>
       <c r="G19" t="s">
         <v>21</v>
       </c>
@@ -1907,22 +1904,6 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" t="s">
-        <v>131</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal PoUomRatioStd {get; set;}</v>
-      </c>
       <c r="G20" t="s">
         <v>27</v>
       </c>
@@ -1952,22 +1933,6 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>168</v>
-      </c>
-      <c r="B21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C21" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="1"/>
-        <v>public decimal PoUomRatio {get; set;}</v>
-      </c>
       <c r="G21" t="s">
         <v>29</v>
       </c>
@@ -2061,61 +2026,218 @@
         <v>public DateTime CreatedOn {get; set;}</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>199</v>
+      </c>
+      <c r="B30" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" ref="F30:F46" si="6">"public " &amp; C30 &amp; IF(D30="Y", "?","") &amp; " "  &amp;  A30 &amp; " {get; set;}"</f>
+        <v>public Guid ProductVariantId {get; set;}</v>
+      </c>
+      <c r="G30" t="s">
+        <v>212</v>
+      </c>
+      <c r="H30" t="s">
+        <v>162</v>
+      </c>
+      <c r="I30" t="s">
+        <v>113</v>
+      </c>
+      <c r="J30" t="s">
+        <v>131</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" ref="L30:L31" si="7">"public " &amp; I30 &amp; IF(J30="Y", "?","") &amp; " "  &amp;  G30 &amp; " {get; set;}"</f>
+        <v>public Guid PromotionId {get; set;}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" t="s">
+        <v>200</v>
+      </c>
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="6"/>
+        <v>public Guid ProductId {get; set;}</v>
+      </c>
+      <c r="G31" t="s">
+        <v>214</v>
+      </c>
+      <c r="H31" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" t="s">
+        <v>116</v>
+      </c>
+      <c r="J31" t="s">
+        <v>131</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="7"/>
+        <v>public string PromotionName {get; set;}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="6"/>
+        <v>public string BarCode {get; set;}</v>
+      </c>
+      <c r="G32" t="s">
+        <v>215</v>
+      </c>
+      <c r="H32" t="s">
+        <v>162</v>
+      </c>
+      <c r="I32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
         <v>208</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="6"/>
+        <v>public decimal? MasterPackQty {get; set;}</v>
+      </c>
+      <c r="G33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="6"/>
+        <v>public decimal? InnerPackQty {get; set;}</v>
+      </c>
+      <c r="G34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>210</v>
+        <v>144</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D35" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="6"/>
+        <v>public decimal? CaseLength {get; set;}</v>
+      </c>
+      <c r="G35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="6"/>
+        <v>public decimal? CaseWidth {get; set;}</v>
+      </c>
+      <c r="G36" t="s">
+        <v>218</v>
+      </c>
+      <c r="H36" t="s">
+        <v>219</v>
+      </c>
+      <c r="I36" t="s">
+        <v>116</v>
+      </c>
+      <c r="J36" t="s">
         <v>131</v>
       </c>
-      <c r="E35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" t="str">
-        <f>"public " &amp; C35 &amp; IF(D35="Y", "?","") &amp; " "  &amp;  A35 &amp; " {get; set;}"</f>
-        <v>public Guid ProductVariantId {get; set;}</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" t="s">
-        <v>139</v>
-      </c>
-      <c r="C36" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" t="s">
-        <v>131</v>
-      </c>
-      <c r="F36" t="str">
-        <f>"public " &amp; C36 &amp; IF(D36="Y", "?","") &amp; " "  &amp;  A36 &amp; " {get; set;}"</f>
-        <v>public string BarCode {get; set;}</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>146</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
         <v>118</v>
@@ -2124,16 +2246,16 @@
         <v>132</v>
       </c>
       <c r="F37" t="str">
-        <f>"public " &amp; C37 &amp; IF(D37="Y", "?","") &amp; " "  &amp;  A37 &amp; " {get; set;}"</f>
-        <v>public decimal? MasterPackQty {get; set;}</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public decimal? CaseHeight {get; set;}</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="C38" t="s">
         <v>118</v>
@@ -2142,16 +2264,16 @@
         <v>132</v>
       </c>
       <c r="F38" t="str">
-        <f>"public " &amp; C38 &amp; IF(D38="Y", "?","") &amp; " "  &amp;  A38 &amp; " {get; set;}"</f>
-        <v>public decimal? InnerPackQty {get; set;}</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public decimal? CaseWeight {get; set;}</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>148</v>
       </c>
       <c r="B39" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
         <v>118</v>
@@ -2160,16 +2282,16 @@
         <v>132</v>
       </c>
       <c r="F39" t="str">
-        <f>"public " &amp; C39 &amp; IF(D39="Y", "?","") &amp; " "  &amp;  A39 &amp; " {get; set;}"</f>
-        <v>public decimal? CaseLength {get; set;}</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public decimal? ProductLength {get; set;}</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="C40" t="s">
         <v>118</v>
@@ -2178,16 +2300,16 @@
         <v>132</v>
       </c>
       <c r="F40" t="str">
-        <f>"public " &amp; C40 &amp; IF(D40="Y", "?","") &amp; " "  &amp;  A40 &amp; " {get; set;}"</f>
-        <v>public decimal? CaseWidth {get; set;}</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public decimal? ProductWidth {get; set;}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>150</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="C41" t="s">
         <v>118</v>
@@ -2196,16 +2318,16 @@
         <v>132</v>
       </c>
       <c r="F41" t="str">
-        <f>"public " &amp; C41 &amp; IF(D41="Y", "?","") &amp; " "  &amp;  A41 &amp; " {get; set;}"</f>
-        <v>public decimal? CaseHeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public decimal? ProductHeight {get; set;}</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="C42" t="s">
         <v>118</v>
@@ -2214,222 +2336,260 @@
         <v>132</v>
       </c>
       <c r="F42" t="str">
-        <f>"public " &amp; C42 &amp; IF(D42="Y", "?","") &amp; " "  &amp;  A42 &amp; " {get; set;}"</f>
-        <v>public decimal? CaseWeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public decimal? ProductWeight {get; set;}</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>152</v>
       </c>
       <c r="B43" t="s">
-        <v>142</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="D43" t="s">
         <v>132</v>
       </c>
       <c r="F43" t="str">
-        <f>"public " &amp; C43 &amp; IF(D43="Y", "?","") &amp; " "  &amp;  A43 &amp; " {get; set;}"</f>
-        <v>public decimal? ProductLength {get; set;}</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public int? LastVendorId {get; set;}</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F44" t="str">
-        <f>"public " &amp; C44 &amp; IF(D44="Y", "?","") &amp; " "  &amp;  A44 &amp; " {get; set;}"</f>
-        <v>public decimal? ProductWidth {get; set;}</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public bool IsSellable {get; set;}</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" t="s">
         <v>154</v>
       </c>
-      <c r="B45" t="s">
-        <v>142</v>
-      </c>
       <c r="C45" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="D45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F45" t="str">
-        <f>"public " &amp; C45 &amp; IF(D45="Y", "?","") &amp; " "  &amp;  A45 &amp; " {get; set;}"</f>
-        <v>public decimal? ProductHeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public bool IsPurchaseable {get; set;}</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B46" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F46" t="str">
-        <f>"public " &amp; C46 &amp; IF(D46="Y", "?","") &amp; " "  &amp;  A46 &amp; " {get; set;}"</f>
-        <v>public decimal? ProductWeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>public bool IsActive {get; set;}</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>156</v>
+        <v>195</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>200</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
         <v>132</v>
       </c>
       <c r="F47" t="str">
-        <f>"public " &amp; C47 &amp; IF(D47="Y", "?","") &amp; " "  &amp;  A47 &amp; " {get; set;}"</f>
-        <v>public int? LastVendorId {get; set;}</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F47:F48" si="8">"public " &amp; C47 &amp; IF(D47="Y", "?","") &amp; " "  &amp;  A47 &amp; " {get; set;}"</f>
+        <v>public Guid? ImageId {get; set;}</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>196</v>
       </c>
       <c r="B48" t="s">
-        <v>158</v>
+        <v>61</v>
       </c>
       <c r="C48" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="D48" t="s">
         <v>131</v>
       </c>
       <c r="F48" t="str">
-        <f>"public " &amp; C48 &amp; IF(D48="Y", "?","") &amp; " "  &amp;  A48 &amp; " {get; set;}"</f>
-        <v>public bool IsSellable {get; set;}</v>
+        <f t="shared" si="8"/>
+        <v>public string SKUCode {get; set;}</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="B49" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" t="s">
-        <v>174</v>
-      </c>
-      <c r="D49" t="s">
-        <v>131</v>
-      </c>
-      <c r="F49" t="str">
-        <f>"public " &amp; C49 &amp; IF(D49="Y", "?","") &amp; " "  &amp;  A49 &amp; " {get; set;}"</f>
-        <v>public bool IsPurchaseable {get; set;}</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>161</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
-      </c>
-      <c r="C50" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" t="s">
-        <v>131</v>
-      </c>
-      <c r="F50" t="str">
-        <f>"public " &amp; C50 &amp; IF(D50="Y", "?","") &amp; " "  &amp;  A50 &amp; " {get; set;}"</f>
-        <v>public bool IsActive {get; set;}</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" t="s">
-        <v>85</v>
-      </c>
-      <c r="D51" t="s">
-        <v>132</v>
-      </c>
-      <c r="F51" t="str">
-        <f t="shared" ref="F51:F52" si="6">"public " &amp; C51 &amp; IF(D51="Y", "?","") &amp; " "  &amp;  A51 &amp; " {get; set;}"</f>
-        <v>public int? ImageId {get; set;}</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" t="s">
+        <v>200</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>199</v>
+      </c>
+      <c r="B55" t="s">
         <v>207</v>
       </c>
-      <c r="B52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" t="s">
-        <v>116</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" t="s">
         <v>131</v>
       </c>
-      <c r="F52" t="str">
-        <f t="shared" si="6"/>
-        <v>public string SKUCode {get; set;}</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="F55" t="str">
+        <f t="shared" ref="F55:F56" si="9">"public " &amp; C55 &amp; IF(D55="Y", "?","") &amp; " "  &amp;  A55 &amp; " {get; set;}"</f>
+        <v>public Guid ProductVariantId {get; set;}</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>195</v>
+      </c>
+      <c r="B56" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" t="s">
+        <v>131</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="9"/>
+        <v>public Guid ImageId {get; set;}</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>226</v>
+      </c>
+      <c r="B65" t="s">
+        <v>227</v>
+      </c>
+      <c r="C65" t="s">
+        <v>113</v>
+      </c>
+      <c r="D65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>223</v>
+      </c>
+      <c r="E68" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" t="s">
-        <v>113</v>
-      </c>
-      <c r="E73" t="s">
-        <v>4</v>
-      </c>
-      <c r="F73" t="str">
-        <f t="shared" ref="F73:F81" si="7">"public " &amp; C73 &amp; " "  &amp;  A73 &amp; " {get; set;}"</f>
-        <v>public Guid AddressID {get; set;}</v>
-      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B74" t="s">
         <v>3</v>
@@ -2438,49 +2598,52 @@
         <v>113</v>
       </c>
       <c r="E74" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="7"/>
-        <v>public Guid UserID {get; set;}</v>
+        <f t="shared" ref="F74:F82" si="10">"public " &amp; C74 &amp; " "  &amp;  A74 &amp; " {get; set;}"</f>
+        <v>public Guid AddressID {get; set;}</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E75" t="s">
         <v>14</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="7"/>
-        <v>public short AddressType {get; set;}</v>
+        <f t="shared" si="10"/>
+        <v>public Guid UserID {get; set;}</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="E76" t="s">
+        <v>14</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="7"/>
-        <v>public string AddressLine1 {get; set;}</v>
+        <f t="shared" si="10"/>
+        <v>public short AddressType {get; set;}</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
@@ -2489,511 +2652,529 @@
         <v>116</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="7"/>
-        <v>public string AddressLine2 {get; set;}</v>
+        <f t="shared" si="10"/>
+        <v>public string AddressLine1 {get; set;}</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
         <v>116</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="7"/>
-        <v>public string City {get; set;}</v>
+        <f t="shared" si="10"/>
+        <v>public string AddressLine2 {get; set;}</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C79" t="s">
         <v>116</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="7"/>
-        <v>public string PostCode {get; set;}</v>
+        <f t="shared" si="10"/>
+        <v>public string City {get; set;}</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
         <v>116</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="7"/>
-        <v>public string State {get; set;}</v>
+        <f t="shared" si="10"/>
+        <v>public string PostCode {get; set;}</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>116</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="10"/>
+        <v>public string State {get; set;}</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>22</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>24</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>115</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E82" t="s">
         <v>14</v>
       </c>
-      <c r="F81" t="str">
-        <f t="shared" si="7"/>
+      <c r="F82" t="str">
+        <f t="shared" si="10"/>
         <v>public short CountryID {get; set;}</v>
       </c>
     </row>
-    <row r="99" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G99" s="1"/>
-    </row>
-    <row r="100" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="M100" s="4" t="s">
+    <row r="104" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G104" s="1"/>
+    </row>
+    <row r="105" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M105" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N100" s="4"/>
-      <c r="O100" s="4"/>
-      <c r="P100" s="4"/>
-    </row>
-    <row r="101" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G101" s="4" t="s">
+      <c r="N105" s="5"/>
+      <c r="O105" s="5"/>
+      <c r="P105" s="5"/>
+    </row>
+    <row r="106" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G106" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
-      <c r="J101" s="4"/>
-      <c r="K101" s="4"/>
-      <c r="M101" s="1" t="s">
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+      <c r="M106" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N101" s="1" t="s">
+      <c r="N106" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O101" s="1"/>
-      <c r="P101" s="1" t="s">
+      <c r="O106" s="1"/>
+      <c r="P106" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G102" t="s">
+    <row r="107" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
         <v>32</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H107" t="s">
         <v>24</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I107" t="s">
         <v>115</v>
       </c>
-      <c r="K102" t="s">
+      <c r="K107" t="s">
         <v>4</v>
       </c>
-      <c r="L102" t="str">
-        <f t="shared" ref="L102:L105" si="8">"public " &amp; I102 &amp; " "  &amp;  G102 &amp; " {get; set;}"</f>
+      <c r="L107" t="str">
+        <f t="shared" ref="L107:L110" si="11">"public " &amp; I107 &amp; " "  &amp;  G107 &amp; " {get; set;}"</f>
         <v>public short CurrencyID {get; set;}</v>
       </c>
-      <c r="M102" t="s">
+      <c r="M107" t="s">
         <v>37</v>
       </c>
-      <c r="N102" t="s">
+      <c r="N107" t="s">
         <v>12</v>
       </c>
-      <c r="O102" t="s">
+      <c r="O107" t="s">
         <v>115</v>
       </c>
-      <c r="Q102" t="str">
-        <f t="shared" ref="Q102:Q126" si="9">"public " &amp; O102 &amp; " "  &amp;  M102 &amp; " {get; set;}"</f>
+      <c r="Q107" t="str">
+        <f t="shared" ref="Q107:Q131" si="12">"public " &amp; O107 &amp; " "  &amp;  M107 &amp; " {get; set;}"</f>
         <v>public short VoucherTypeID {get; set;}</v>
       </c>
     </row>
-    <row r="103" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G103" t="s">
+    <row r="108" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
         <v>30</v>
       </c>
-      <c r="H103" t="s">
+      <c r="H108" t="s">
         <v>34</v>
       </c>
-      <c r="I103" t="s">
-        <v>116</v>
-      </c>
-      <c r="L103" t="str">
-        <f t="shared" si="8"/>
+      <c r="I108" t="s">
+        <v>116</v>
+      </c>
+      <c r="L108" t="str">
+        <f t="shared" si="11"/>
         <v>public string CurrencyCode {get; set;}</v>
       </c>
-      <c r="M103" t="s">
+      <c r="M108" t="s">
         <v>60</v>
       </c>
-      <c r="N103" t="s">
+      <c r="N108" t="s">
         <v>62</v>
       </c>
-      <c r="O103" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q103" t="str">
-        <f t="shared" si="9"/>
+      <c r="O108" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q108" t="str">
+        <f t="shared" si="12"/>
         <v>public string VoucherType {get; set;}</v>
       </c>
     </row>
-    <row r="104" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G104" t="s">
+    <row r="109" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
         <v>33</v>
       </c>
-      <c r="H104" t="s">
+      <c r="H109" t="s">
         <v>35</v>
       </c>
-      <c r="I104" t="s">
-        <v>116</v>
-      </c>
-      <c r="L104" t="str">
-        <f t="shared" si="8"/>
+      <c r="I109" t="s">
+        <v>116</v>
+      </c>
+      <c r="L109" t="str">
+        <f t="shared" si="11"/>
         <v>public string CurrencySymbol {get; set;}</v>
       </c>
-      <c r="M104" t="s">
+      <c r="M109" t="s">
         <v>1</v>
       </c>
-      <c r="N104" t="s">
+      <c r="N109" t="s">
         <v>61</v>
       </c>
-      <c r="O104" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q104" t="str">
-        <f t="shared" si="9"/>
+      <c r="O109" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q109" t="str">
+        <f t="shared" si="12"/>
         <v>public string Description {get; set;}</v>
       </c>
     </row>
-    <row r="105" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G105" t="s">
+    <row r="110" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
         <v>31</v>
       </c>
-      <c r="H105" t="s">
+      <c r="H110" t="s">
         <v>25</v>
       </c>
-      <c r="I105" t="s">
-        <v>116</v>
-      </c>
-      <c r="L105" t="str">
-        <f t="shared" si="8"/>
+      <c r="I110" t="s">
+        <v>116</v>
+      </c>
+      <c r="L110" t="str">
+        <f t="shared" si="11"/>
         <v>public string Currency {get; set;}</v>
       </c>
     </row>
-    <row r="107" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="M107" s="4" t="s">
+    <row r="112" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M112" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="N107" s="4"/>
-      <c r="O107" s="4"/>
-      <c r="P107" s="4"/>
-    </row>
-    <row r="108" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="M108" s="1" t="s">
+      <c r="N112" s="5"/>
+      <c r="O112" s="5"/>
+      <c r="P112" s="5"/>
+    </row>
+    <row r="113" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M113" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N108" s="1" t="s">
+      <c r="N113" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O108" s="1"/>
-      <c r="P108" s="1" t="s">
+      <c r="O113" s="1"/>
+      <c r="P113" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G109" s="4" t="s">
+    <row r="114" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G114" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H109" s="4"/>
-      <c r="I109" s="4"/>
-      <c r="J109" s="4"/>
-      <c r="K109" s="4"/>
-      <c r="M109" t="s">
+      <c r="H114" s="5"/>
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="5"/>
+      <c r="M114" t="s">
         <v>44</v>
       </c>
-      <c r="N109" t="s">
+      <c r="N114" t="s">
         <v>3</v>
       </c>
-      <c r="O109" t="s">
+      <c r="O114" t="s">
         <v>113</v>
       </c>
-      <c r="Q109" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q114" t="str">
+        <f t="shared" si="12"/>
         <v>public Guid AccountID {get; set;}</v>
       </c>
     </row>
-    <row r="110" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="G110" s="1" t="s">
+    <row r="115" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G115" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H110" s="1" t="s">
+      <c r="H115" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I110" s="1"/>
-      <c r="J110" s="1"/>
-      <c r="K110" s="1" t="s">
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M110" t="s">
+      <c r="M115" t="s">
         <v>0</v>
       </c>
-      <c r="N110" t="s">
+      <c r="N115" t="s">
         <v>3</v>
       </c>
-      <c r="O110" t="s">
+      <c r="O115" t="s">
         <v>113</v>
       </c>
-      <c r="P110" t="s">
+      <c r="P115" t="s">
         <v>14</v>
       </c>
-      <c r="Q110" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q115" t="str">
+        <f t="shared" si="12"/>
         <v>public Guid UserID {get; set;}</v>
       </c>
     </row>
-    <row r="111" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="M111" t="s">
+    <row r="116" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M116" t="s">
         <v>64</v>
       </c>
-      <c r="N111" t="s">
+      <c r="N116" t="s">
         <v>62</v>
       </c>
-      <c r="O111" t="s">
-        <v>116</v>
-      </c>
-      <c r="P111" t="s">
+      <c r="O116" t="s">
+        <v>116</v>
+      </c>
+      <c r="P116" t="s">
         <v>83</v>
       </c>
-      <c r="Q111" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q116" t="str">
+        <f t="shared" si="12"/>
         <v>public string Account {get; set;}</v>
       </c>
     </row>
-    <row r="112" spans="7:17" x14ac:dyDescent="0.25">
-      <c r="M112" t="s">
+    <row r="117" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M117" t="s">
         <v>41</v>
       </c>
-      <c r="N112" t="s">
+      <c r="N117" t="s">
         <v>65</v>
       </c>
-      <c r="O112" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q112" t="str">
-        <f t="shared" si="9"/>
+      <c r="O117" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q117" t="str">
+        <f t="shared" si="12"/>
         <v>public string CrDr {get; set;}</v>
       </c>
     </row>
-    <row r="113" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M113" t="s">
+    <row r="118" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M118" t="s">
         <v>1</v>
       </c>
-      <c r="N113" t="s">
+      <c r="N118" t="s">
         <v>61</v>
       </c>
-      <c r="O113" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q113" t="str">
-        <f t="shared" si="9"/>
+      <c r="O118" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q118" t="str">
+        <f t="shared" si="12"/>
         <v>public string Description {get; set;}</v>
       </c>
     </row>
-    <row r="114" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M114" t="s">
+    <row r="119" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M119" t="s">
         <v>66</v>
       </c>
-      <c r="N114" t="s">
+      <c r="N119" t="s">
         <v>12</v>
       </c>
-      <c r="O114" t="s">
+      <c r="O119" t="s">
         <v>115</v>
       </c>
-      <c r="Q114" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q119" t="str">
+        <f t="shared" si="12"/>
         <v>public short ParentAccountID {get; set;}</v>
       </c>
     </row>
-    <row r="117" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M117" s="4" t="s">
+    <row r="122" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M122" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="N117" s="4" t="s">
+      <c r="N122" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O117" s="4"/>
-      <c r="P117" s="4"/>
-    </row>
-    <row r="118" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M118" t="s">
+      <c r="O122" s="5"/>
+      <c r="P122" s="5"/>
+    </row>
+    <row r="123" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M123" t="s">
         <v>81</v>
       </c>
-      <c r="N118" t="s">
+      <c r="N123" t="s">
         <v>3</v>
       </c>
-      <c r="O118" t="s">
+      <c r="O123" t="s">
         <v>113</v>
       </c>
-      <c r="P118" t="s">
+      <c r="P123" t="s">
         <v>4</v>
       </c>
-      <c r="Q118" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q123" t="str">
+        <f t="shared" si="12"/>
         <v>public Guid AccountAddressID {get; set;}</v>
       </c>
     </row>
-    <row r="119" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M119" t="s">
+    <row r="124" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M124" t="s">
         <v>44</v>
       </c>
-      <c r="N119" t="s">
+      <c r="N124" t="s">
         <v>3</v>
       </c>
-      <c r="O119" t="s">
+      <c r="O124" t="s">
         <v>113</v>
       </c>
-      <c r="P119" t="s">
+      <c r="P124" t="s">
         <v>14</v>
       </c>
-      <c r="Q119" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q124" t="str">
+        <f t="shared" si="12"/>
         <v>public Guid AccountID {get; set;}</v>
       </c>
     </row>
-    <row r="120" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M120" t="s">
+    <row r="125" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M125" t="s">
         <v>15</v>
       </c>
-      <c r="N120" t="s">
+      <c r="N125" t="s">
         <v>12</v>
       </c>
-      <c r="O120" t="s">
+      <c r="O125" t="s">
         <v>115</v>
       </c>
-      <c r="P120" t="s">
+      <c r="P125" t="s">
         <v>14</v>
       </c>
-      <c r="Q120" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q125" t="str">
+        <f t="shared" si="12"/>
         <v>public short AddressType {get; set;}</v>
       </c>
     </row>
-    <row r="121" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M121" t="s">
+    <row r="126" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M126" t="s">
         <v>16</v>
       </c>
-      <c r="N121" t="s">
+      <c r="N126" t="s">
         <v>5</v>
       </c>
-      <c r="O121" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q121" t="str">
-        <f t="shared" si="9"/>
+      <c r="O126" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q126" t="str">
+        <f t="shared" si="12"/>
         <v>public string AddressLine1 {get; set;}</v>
       </c>
     </row>
-    <row r="122" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M122" t="s">
+    <row r="127" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M127" t="s">
         <v>17</v>
       </c>
-      <c r="N122" t="s">
+      <c r="N127" t="s">
         <v>5</v>
       </c>
-      <c r="O122" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q122" t="str">
-        <f t="shared" si="9"/>
+      <c r="O127" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q127" t="str">
+        <f t="shared" si="12"/>
         <v>public string AddressLine2 {get; set;}</v>
       </c>
     </row>
-    <row r="123" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M123" t="s">
+    <row r="128" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="M128" t="s">
         <v>18</v>
       </c>
-      <c r="N123" t="s">
+      <c r="N128" t="s">
         <v>8</v>
       </c>
-      <c r="O123" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q123" t="str">
-        <f t="shared" si="9"/>
+      <c r="O128" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q128" t="str">
+        <f t="shared" si="12"/>
         <v>public string City {get; set;}</v>
       </c>
     </row>
-    <row r="124" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M124" t="s">
+    <row r="129" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M129" t="s">
         <v>19</v>
       </c>
-      <c r="N124" t="s">
+      <c r="N129" t="s">
         <v>23</v>
       </c>
-      <c r="O124" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q124" t="str">
-        <f t="shared" si="9"/>
+      <c r="O129" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q129" t="str">
+        <f t="shared" si="12"/>
         <v>public string PostCode {get; set;}</v>
       </c>
     </row>
-    <row r="125" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M125" t="s">
+    <row r="130" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M130" t="s">
         <v>20</v>
       </c>
-      <c r="N125" t="s">
+      <c r="N130" t="s">
         <v>8</v>
       </c>
-      <c r="O125" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q125" t="str">
-        <f t="shared" si="9"/>
+      <c r="O130" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q130" t="str">
+        <f t="shared" si="12"/>
         <v>public string State {get; set;}</v>
       </c>
     </row>
-    <row r="126" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M126" t="s">
+    <row r="131" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M131" t="s">
         <v>22</v>
       </c>
-      <c r="N126" t="s">
+      <c r="N131" t="s">
         <v>24</v>
       </c>
-      <c r="O126" t="s">
+      <c r="O131" t="s">
         <v>115</v>
       </c>
-      <c r="P126" t="s">
+      <c r="P131" t="s">
         <v>14</v>
       </c>
-      <c r="Q126" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q131" t="str">
+        <f t="shared" si="12"/>
         <v>public short CountryID {get; set;}</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="M117:P117"/>
-    <mergeCell ref="G109:K109"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="M100:P100"/>
-    <mergeCell ref="M107:P107"/>
-    <mergeCell ref="G101:K101"/>
-    <mergeCell ref="A72:E72"/>
+  <mergeCells count="16">
+    <mergeCell ref="A73:E73"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A29:F29"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="M122:P122"/>
+    <mergeCell ref="G114:K114"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="M105:P105"/>
+    <mergeCell ref="M112:P112"/>
+    <mergeCell ref="G106:K106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added MVC only project and removed MVC + API Product for web client
</commit_message>
<xml_diff>
--- a/Functional/InventoryEntities.xlsx
+++ b/Functional/InventoryEntities.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="228">
   <si>
     <t>UserID</t>
   </si>
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:Q131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="F3" sqref="F3:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2426,7 +2426,7 @@
         <v>132</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" ref="F47:F48" si="8">"public " &amp; C47 &amp; IF(D47="Y", "?","") &amp; " "  &amp;  A47 &amp; " {get; set;}"</f>
+        <f t="shared" ref="F47:F52" si="8">"public " &amp; C47 &amp; IF(D47="Y", "?","") &amp; " "  &amp;  A47 &amp; " {get; set;}"</f>
         <v>public Guid? ImageId {get; set;}</v>
       </c>
     </row>
@@ -2455,6 +2455,13 @@
       <c r="B49" t="s">
         <v>208</v>
       </c>
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="8"/>
+        <v>public decimal LastPurchasePrice {get; set;}</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -2463,6 +2470,13 @@
       <c r="B50" t="s">
         <v>208</v>
       </c>
+      <c r="C50" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="8"/>
+        <v>public decimal BasePrice {get; set;}</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -2471,6 +2485,13 @@
       <c r="B51" t="s">
         <v>208</v>
       </c>
+      <c r="C51" t="s">
+        <v>118</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="8"/>
+        <v>public decimal ShelfPrice {get; set;}</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -2481,6 +2502,10 @@
       </c>
       <c r="C52" t="s">
         <v>113</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="8"/>
+        <v>public Guid PromotionId {get; set;}</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3159,6 +3184,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="M122:P122"/>
+    <mergeCell ref="G114:K114"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="M105:P105"/>
+    <mergeCell ref="M112:P112"/>
+    <mergeCell ref="G106:K106"/>
     <mergeCell ref="A73:E73"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G7:K7"/>
@@ -3168,13 +3200,6 @@
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="G29:L29"/>
     <mergeCell ref="A64:F64"/>
-    <mergeCell ref="M122:P122"/>
-    <mergeCell ref="G114:K114"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="M105:P105"/>
-    <mergeCell ref="M112:P112"/>
-    <mergeCell ref="G106:K106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change in entity excel file
</commit_message>
<xml_diff>
--- a/Functional/InventoryEntities.xlsx
+++ b/Functional/InventoryEntities.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="268">
   <si>
     <t>UserID</t>
   </si>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>AccountAddress</t>
-  </si>
-  <si>
-    <t>UserAddress</t>
   </si>
   <si>
     <t>AccountAddressID</t>
@@ -450,12 +447,6 @@
     <t>ReorderQuantity</t>
   </si>
   <si>
-    <t>MasterPackQty</t>
-  </si>
-  <si>
-    <t>InnerPackQty</t>
-  </si>
-  <si>
     <t>CaseLength</t>
   </si>
   <si>
@@ -636,9 +627,6 @@
     <t>SalesOrderUnitId</t>
   </si>
   <si>
-    <t>UnitId</t>
-  </si>
-  <si>
     <t>PurchaseOrderUnitId</t>
   </si>
   <si>
@@ -706,6 +694,138 @@
   </si>
   <si>
     <t>UniquIdentifier</t>
+  </si>
+  <si>
+    <t>ProductVariantType</t>
+  </si>
+  <si>
+    <t>PurchaseOrderVolume</t>
+  </si>
+  <si>
+    <t>SalesOrderVolume</t>
+  </si>
+  <si>
+    <t>VolumeMeasureId</t>
+  </si>
+  <si>
+    <t>PrimaryKey</t>
+  </si>
+  <si>
+    <t>VolumeMeasureName</t>
+  </si>
+  <si>
+    <t>ShortName</t>
+  </si>
+  <si>
+    <t>VolumeMeasureMapping</t>
+  </si>
+  <si>
+    <t>VolumeMeasureMappingId</t>
+  </si>
+  <si>
+    <t>PrimaryVMId</t>
+  </si>
+  <si>
+    <t>SecondaryVMId</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>decimal(10,2)</t>
+  </si>
+  <si>
+    <t>CategoryId</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>Category Description</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>SubCategoryName</t>
+  </si>
+  <si>
+    <t>SubCategory Description</t>
+  </si>
+  <si>
+    <t>CategorySubCategoryMapId</t>
+  </si>
+  <si>
+    <t>CategorySubCategoryMap</t>
+  </si>
+  <si>
+    <t>ImageFile</t>
+  </si>
+  <si>
+    <t>ImageFileId</t>
+  </si>
+  <si>
+    <t>ImageUrl</t>
+  </si>
+  <si>
+    <t>varchar(300)</t>
+  </si>
+  <si>
+    <t>ImageType</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>ImageData</t>
+  </si>
+  <si>
+    <t>varbinary(max)</t>
+  </si>
+  <si>
+    <t>byte[]</t>
+  </si>
+  <si>
+    <t>ProductAttribute</t>
+  </si>
+  <si>
+    <t>ProductAttributeId</t>
+  </si>
+  <si>
+    <t>AttributeName</t>
+  </si>
+  <si>
+    <t>AttributeDescription</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>AgentName</t>
+  </si>
+  <si>
+    <t>AgentContactNo</t>
+  </si>
+  <si>
+    <t>AgentEmailId</t>
+  </si>
+  <si>
+    <t>AddressMapId</t>
+  </si>
+  <si>
+    <t>eg. UserId / AgentId</t>
+  </si>
+  <si>
+    <t>Address Type Enum</t>
+  </si>
+  <si>
+    <t>DefaultAddress</t>
   </si>
 </sst>
 </file>
@@ -1100,123 +1220,123 @@
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" t="s">
         <v>164</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>165</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>166</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2" t="s">
         <v>167</v>
-      </c>
-      <c r="G2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2" t="s">
-        <v>169</v>
-      </c>
-      <c r="I2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" t="s">
         <v>172</v>
       </c>
-      <c r="C3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" t="s">
-        <v>175</v>
-      </c>
       <c r="H3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1226,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q131"/>
+  <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F16"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,7 +1369,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1263,12 +1383,14 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
       <c r="M1" s="5" t="s">
         <v>38</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1278,16 +1400,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
@@ -1296,10 +1418,10 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>1</v>
@@ -1317,16 +1439,16 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F3" t="str">
         <f>"public " &amp; C3 &amp; IF(D3="Y", "?","") &amp; " "  &amp;  A3 &amp; " {get; set;}"</f>
@@ -1339,7 +1461,7 @@
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K3" t="s">
         <v>4</v>
@@ -1355,7 +1477,7 @@
         <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q3" t="str">
         <f t="shared" ref="Q3:Q10" si="0">"public " &amp; O3 &amp; " "  &amp;  M3 &amp; " {get; set;}"</f>
@@ -1364,19 +1486,19 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F16" si="1">"public " &amp; C4 &amp; IF(D4="Y", "?","") &amp; " "  &amp;  A4 &amp; " {get; set;}"</f>
+        <f t="shared" ref="F4:F15" si="1">"public " &amp; C4 &amp; IF(D4="Y", "?","") &amp; " "  &amp;  A4 &amp; " {get; set;}"</f>
         <v>public int ItemType {get; set;}</v>
       </c>
       <c r="G4" t="s">
@@ -1386,7 +1508,7 @@
         <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ref="L4:L5" si="2">"public " &amp; I4 &amp; " "  &amp;  G4 &amp; " {get; set;}"</f>
@@ -1399,7 +1521,7 @@
         <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="0"/>
@@ -1408,16 +1530,16 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1430,7 +1552,7 @@
         <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="2"/>
@@ -1443,7 +1565,7 @@
         <v>7</v>
       </c>
       <c r="O5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
@@ -1455,13 +1577,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -1474,7 +1596,7 @@
         <v>40</v>
       </c>
       <c r="O6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
@@ -1483,16 +1605,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -1505,6 +1627,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
       <c r="M7" t="s">
         <v>41</v>
       </c>
@@ -1512,7 +1635,7 @@
         <v>42</v>
       </c>
       <c r="O7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P7" t="s">
         <v>43</v>
@@ -1524,20 +1647,20 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>243</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
-        <v>public Guid SubCategoryId {get; set;}</v>
+        <v>public Guid CategorySubCategoryMapId {get; set;}</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>6</v>
@@ -1557,7 +1680,7 @@
         <v>50</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
@@ -1566,16 +1689,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" t="s">
         <v>139</v>
       </c>
-      <c r="B9" t="s">
-        <v>140</v>
-      </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -1588,7 +1711,7 @@
         <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K9" t="s">
         <v>4</v>
@@ -1604,7 +1727,7 @@
         <v>58</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="0"/>
@@ -1613,16 +1736,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -1635,7 +1758,7 @@
         <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ref="L10:L11" si="3">"public " &amp; I10 &amp; " "  &amp;  G10 &amp; " {get; set;}"</f>
@@ -1648,7 +1771,7 @@
         <v>7</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="0"/>
@@ -1657,20 +1780,20 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
-        <v>public Guid UnitId {get; set;}</v>
+        <v>public int LastModifiedBy {get; set;}</v>
       </c>
       <c r="G11" t="s">
         <v>1</v>
@@ -1679,7 +1802,7 @@
         <v>8</v>
       </c>
       <c r="I11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="3"/>
@@ -1688,56 +1811,56 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
-        <v>public int LastModifiedBy {get; set;}</v>
+        <v>public DateTime LastModifiedOn {get; set;}</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" t="s">
         <v>159</v>
       </c>
-      <c r="B13" t="s">
-        <v>156</v>
-      </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
         <v>131</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
-        <v>public DateTime LastModifiedOn {get; set;}</v>
+        <v>public Guid? ImageId {get; set;}</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
-        <v>public Guid? ImageId {get; set;}</v>
+        <v>public Guid SalesOrderUnitId {get; set;}</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>46</v>
@@ -1745,23 +1868,24 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
-        <v>public Guid SalesOrderUnitId {get; set;}</v>
+        <v>public Guid PurchaseOrderUnitId {get; set;}</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>6</v>
@@ -1775,22 +1899,6 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="1"/>
-        <v>public Guid PurchaseOrderUnitId {get; set;}</v>
-      </c>
       <c r="G16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1798,6 +1906,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="2" t="s">
         <v>47</v>
       </c>
@@ -1805,7 +1914,7 @@
         <v>3</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" t="str">
@@ -1813,7 +1922,7 @@
         <v>public Guid VoucherDetailID {get; set;}</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1832,7 +1941,7 @@
         <v>3</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>14</v>
@@ -1842,7 +1951,7 @@
         <v>public Guid VoucherID {get; set;}</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
         <v>22</v>
       </c>
@@ -1850,7 +1959,7 @@
         <v>24</v>
       </c>
       <c r="I18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K18" t="s">
         <v>4</v>
@@ -1866,7 +1975,7 @@
         <v>59</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" t="str">
@@ -1874,7 +1983,7 @@
         <v>public string Item {get; set;}</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
         <v>21</v>
       </c>
@@ -1882,7 +1991,7 @@
         <v>25</v>
       </c>
       <c r="I19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="5"/>
@@ -1895,7 +2004,7 @@
         <v>58</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" t="str">
@@ -1903,7 +2012,7 @@
         <v>public decimal Quantity {get; set;}</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
         <v>27</v>
       </c>
@@ -1911,7 +2020,7 @@
         <v>28</v>
       </c>
       <c r="I20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="5"/>
@@ -1924,7 +2033,7 @@
         <v>58</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" t="str">
@@ -1932,7 +2041,7 @@
         <v>public decimal UnitPrice {get; set;}</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
         <v>29</v>
       </c>
@@ -1940,7 +2049,7 @@
         <v>28</v>
       </c>
       <c r="I21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="5"/>
@@ -1953,7 +2062,7 @@
         <v>3</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" t="str">
@@ -1961,7 +2070,7 @@
         <v>public Guid AccountID {get; set;}</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>32</v>
       </c>
@@ -1969,7 +2078,7 @@
         <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="5"/>
@@ -1982,7 +2091,7 @@
         <v>58</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>55</v>
@@ -1992,7 +2101,7 @@
         <v>public decimal Volume {get; set;}</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M23" s="2" t="s">
         <v>54</v>
       </c>
@@ -2000,7 +2109,7 @@
         <v>28</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>56</v>
@@ -2010,7 +2119,7 @@
         <v>public string VolumeMeasure {get; set;}</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M24" s="2" t="s">
         <v>45</v>
       </c>
@@ -2018,7 +2127,7 @@
         <v>7</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" t="str">
@@ -2026,737 +2135,1306 @@
         <v>public DateTime CreatedOn {get; set;}</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" t="s">
         <v>197</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" ref="F29:F45" si="6">"public " &amp; C29 &amp; IF(D29="Y", "?","") &amp; " "  &amp;  A29 &amp; " {get; set;}"</f>
+        <v>public Guid ProductVariantId {get; set;}</v>
+      </c>
       <c r="G29" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>199</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>131</v>
-      </c>
-      <c r="E30" t="s">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="F30:F46" si="6">"public " &amp; C30 &amp; IF(D30="Y", "?","") &amp; " "  &amp;  A30 &amp; " {get; set;}"</f>
-        <v>public Guid ProductVariantId {get; set;}</v>
+        <f t="shared" si="6"/>
+        <v>public Guid ProductId {get; set;}</v>
       </c>
       <c r="G30" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H30" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ref="L30:L31" si="7">"public " &amp; I30 &amp; IF(J30="Y", "?","") &amp; " "  &amp;  G30 &amp; " {get; set;}"</f>
         <v>public Guid PromotionId {get; set;}</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>227</v>
+      </c>
+      <c r="N30" t="s">
+        <v>159</v>
+      </c>
+      <c r="O30" t="s">
+        <v>112</v>
+      </c>
+      <c r="P30" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" ref="Q30:Q32" si="8">"public " &amp; O30 &amp; " "  &amp;  M30 &amp; " {get; set;}"</f>
+        <v>public Guid VolumeMeasureId {get; set;}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>137</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="D31" t="s">
+        <v>130</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="6"/>
-        <v>public Guid ProductId {get; set;}</v>
+        <v>public string BarCode {get; set;}</v>
       </c>
       <c r="G31" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H31" t="s">
         <v>59</v>
       </c>
       <c r="I31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="7"/>
         <v>public string PromotionName {get; set;}</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>229</v>
+      </c>
+      <c r="N31" t="s">
+        <v>59</v>
+      </c>
+      <c r="O31" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="8"/>
+        <v>public string VolumeMeasureName {get; set;}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>225</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="6"/>
-        <v>public string BarCode {get; set;}</v>
+        <v>public decimal PurchaseOrderVolume {get; set;}</v>
       </c>
       <c r="G32" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="M32" t="s">
+        <v>230</v>
+      </c>
+      <c r="N32" t="s">
+        <v>28</v>
+      </c>
+      <c r="O32" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" si="8"/>
+        <v>public string ShortName {get; set;}</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>226</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? MasterPackQty {get; set;}</v>
+        <v>public decimal SalesOrderVolume {get; set;}</v>
       </c>
       <c r="G33" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? InnerPackQty {get; set;}</v>
+        <v>public decimal? CaseLength {get; set;}</v>
       </c>
       <c r="G34" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? CaseLength {get; set;}</v>
+        <v>public decimal? CaseWidth {get; set;}</v>
       </c>
       <c r="G35" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? CaseWidth {get; set;}</v>
+        <v>public decimal? CaseHeight {get; set;}</v>
       </c>
       <c r="G36" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H36" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" t="s">
-        <v>208</v>
-      </c>
-      <c r="C37" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" t="s">
-        <v>132</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? CaseHeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public decimal? CaseWeight {get; set;}</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? CaseWeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public decimal? ProductLength {get; set;}</v>
+      </c>
+      <c r="M38" t="s">
+        <v>232</v>
+      </c>
+      <c r="N38" t="s">
+        <v>159</v>
+      </c>
+      <c r="O38" t="s">
+        <v>112</v>
+      </c>
+      <c r="P38" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" ref="Q38:Q40" si="9">"public " &amp; O38 &amp; " "  &amp;  M38 &amp; " {get; set;}"</f>
+        <v>public Guid VolumeMeasureMappingId {get; set;}</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? ProductLength {get; set;}</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public decimal? ProductWidth {get; set;}</v>
+      </c>
+      <c r="M39" t="s">
+        <v>233</v>
+      </c>
+      <c r="N39" t="s">
+        <v>159</v>
+      </c>
+      <c r="O39" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="9"/>
+        <v>public Guid PrimaryVMId {get; set;}</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? ProductWidth {get; set;}</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public decimal? ProductHeight {get; set;}</v>
+      </c>
+      <c r="M40" t="s">
+        <v>234</v>
+      </c>
+      <c r="N40" t="s">
+        <v>159</v>
+      </c>
+      <c r="O40" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="9"/>
+        <v>public Guid SecondaryVMId {get; set;}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? ProductHeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public decimal? ProductWeight {get; set;}</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" t="s">
+        <v>235</v>
+      </c>
+      <c r="N41" t="s">
+        <v>236</v>
+      </c>
+      <c r="O41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="6"/>
-        <v>public decimal? ProductWeight {get; set;}</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public Guid? LastVendorId {get; set;}</v>
+      </c>
+      <c r="G42" t="s">
+        <v>246</v>
+      </c>
+      <c r="H42" t="s">
+        <v>159</v>
+      </c>
+      <c r="I42" t="s">
+        <v>112</v>
+      </c>
+      <c r="J42" t="s">
+        <v>130</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" ref="L42:L45" si="10">"public " &amp; I42 &amp; IF(J42="Y", "?","") &amp; " "  &amp;  G42 &amp; " {get; set;}"</f>
+        <v>public Guid ImageFileId {get; set;}</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="6"/>
-        <v>public int? LastVendorId {get; set;}</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public bool IsSellable {get; set;}</v>
+      </c>
+      <c r="G43" t="s">
+        <v>247</v>
+      </c>
+      <c r="H43" t="s">
+        <v>248</v>
+      </c>
+      <c r="I43" t="s">
+        <v>115</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="10"/>
+        <v>public string ImageUrl {get; set;}</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="6"/>
-        <v>public bool IsSellable {get; set;}</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public bool IsPurchaseable {get; set;}</v>
+      </c>
+      <c r="G44" t="s">
+        <v>249</v>
+      </c>
+      <c r="H44" t="s">
+        <v>250</v>
+      </c>
+      <c r="I44" t="s">
+        <v>115</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="10"/>
+        <v>public string ImageType {get; set;}</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B45" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="6"/>
-        <v>public bool IsPurchaseable {get; set;}</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>public bool IsActive {get; set;}</v>
+      </c>
+      <c r="G45" t="s">
+        <v>251</v>
+      </c>
+      <c r="H45" t="s">
+        <v>252</v>
+      </c>
+      <c r="I45" t="s">
+        <v>253</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="10"/>
+        <v>public byte[] ImageData {get; set;}</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B46" t="s">
-        <v>154</v>
+        <v>197</v>
       </c>
       <c r="C46" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="D46" t="s">
         <v>131</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="6"/>
-        <v>public bool IsActive {get; set;}</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F46:F52" si="11">"public " &amp; C46 &amp; IF(D46="Y", "?","") &amp; " "  &amp;  A46 &amp; " {get; set;}"</f>
+        <v>public Guid? ImageId {get; set;}</v>
+      </c>
+      <c r="M46" t="s">
+        <v>237</v>
+      </c>
+      <c r="N46" t="s">
+        <v>159</v>
+      </c>
+      <c r="O46" t="s">
+        <v>112</v>
+      </c>
+      <c r="P46" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q46" t="str">
+        <f t="shared" ref="Q46:Q48" si="12">"public " &amp; O46 &amp; " "  &amp;  M46 &amp; " {get; set;}"</f>
+        <v>public Guid CategoryId {get; set;}</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>61</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D47" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" ref="F47:F52" si="8">"public " &amp; C47 &amp; IF(D47="Y", "?","") &amp; " "  &amp;  A47 &amp; " {get; set;}"</f>
-        <v>public Guid? ImageId {get; set;}</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>public string SKUCode {get; set;}</v>
+      </c>
+      <c r="M47" t="s">
+        <v>238</v>
+      </c>
+      <c r="N47" t="s">
+        <v>59</v>
+      </c>
+      <c r="O47" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q47" t="str">
+        <f t="shared" si="12"/>
+        <v>public string CategoryName {get; set;}</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>204</v>
       </c>
       <c r="C48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="8"/>
-        <v>public string SKUCode {get; set;}</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>public decimal LastPurchasePrice {get; set;}</v>
+      </c>
+      <c r="M48" t="s">
+        <v>239</v>
+      </c>
+      <c r="N48" t="s">
+        <v>215</v>
+      </c>
+      <c r="O48" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q48" t="str">
+        <f t="shared" si="12"/>
+        <v>public string Category Description {get; set;}</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>209</v>
       </c>
       <c r="B49" t="s">
+        <v>204</v>
+      </c>
+      <c r="C49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="11"/>
+        <v>public decimal BasePrice {get; set;}</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D50" t="s">
+        <v>130</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="11"/>
+        <v>public decimal ShelfPrice {get; set;}</v>
+      </c>
+      <c r="G50" t="s">
+        <v>255</v>
+      </c>
+      <c r="H50" t="s">
+        <v>159</v>
+      </c>
+      <c r="I50" t="s">
+        <v>112</v>
+      </c>
+      <c r="J50" t="s">
+        <v>130</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" ref="L50:L52" si="13">"public " &amp; I50 &amp; IF(J50="Y", "?","") &amp; " "  &amp;  G50 &amp; " {get; set;}"</f>
+        <v>public Guid ProductAttributeId {get; set;}</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>208</v>
       </c>
-      <c r="C49" t="s">
-        <v>118</v>
-      </c>
-      <c r="F49" t="str">
-        <f t="shared" si="8"/>
-        <v>public decimal LastPurchasePrice {get; set;}</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>213</v>
-      </c>
-      <c r="B50" t="s">
-        <v>208</v>
-      </c>
-      <c r="C50" t="s">
-        <v>118</v>
-      </c>
-      <c r="F50" t="str">
-        <f t="shared" si="8"/>
-        <v>public decimal BasePrice {get; set;}</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>210</v>
-      </c>
       <c r="B51" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="D51" t="s">
+        <v>131</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="8"/>
-        <v>public decimal ShelfPrice {get; set;}</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>public Guid? PromotionId {get; set;}</v>
+      </c>
+      <c r="G51" t="s">
+        <v>256</v>
+      </c>
+      <c r="H51" t="s">
+        <v>250</v>
+      </c>
+      <c r="I51" t="s">
+        <v>115</v>
+      </c>
+      <c r="J51" t="s">
+        <v>130</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="13"/>
+        <v>public string AttributeName {get; set;}</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="B52" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C52" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="D52" t="s">
+        <v>130</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="8"/>
-        <v>public Guid PromotionId {get; set;}</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+        <f t="shared" si="11"/>
+        <v>public Guid ProductVariantType {get; set;}</v>
+      </c>
+      <c r="G52" t="s">
+        <v>257</v>
+      </c>
+      <c r="H52" t="s">
+        <v>215</v>
+      </c>
+      <c r="I52" t="s">
+        <v>115</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="13"/>
+        <v>public string AttributeDescription {get; set;}</v>
+      </c>
+      <c r="M52" t="s">
         <v>199</v>
       </c>
-      <c r="B55" t="s">
-        <v>207</v>
-      </c>
-      <c r="C55" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" t="s">
-        <v>131</v>
-      </c>
-      <c r="F55" t="str">
-        <f t="shared" ref="F55:F56" si="9">"public " &amp; C55 &amp; IF(D55="Y", "?","") &amp; " "  &amp;  A55 &amp; " {get; set;}"</f>
+      <c r="N52" t="s">
+        <v>159</v>
+      </c>
+      <c r="O52" t="s">
+        <v>112</v>
+      </c>
+      <c r="P52" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q52" t="str">
+        <f t="shared" ref="Q52:Q54" si="14">"public " &amp; O52 &amp; " "  &amp;  M52 &amp; " {get; set;}"</f>
+        <v>public Guid SubCategoryId {get; set;}</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M53" t="s">
+        <v>241</v>
+      </c>
+      <c r="N53" t="s">
+        <v>59</v>
+      </c>
+      <c r="O53" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q53" t="str">
+        <f t="shared" si="14"/>
+        <v>public string SubCategoryName {get; set;}</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M54" t="s">
+        <v>242</v>
+      </c>
+      <c r="N54" t="s">
+        <v>215</v>
+      </c>
+      <c r="O54" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q54" t="str">
+        <f t="shared" si="14"/>
+        <v>public string SubCategory Description {get; set;}</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>196</v>
+      </c>
+      <c r="B56" t="s">
+        <v>203</v>
+      </c>
+      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" t="s">
+        <v>130</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" ref="F56:F57" si="15">"public " &amp; C56 &amp; IF(D56="Y", "?","") &amp; " "  &amp;  A56 &amp; " {get; set;}"</f>
         <v>public Guid ProductVariantId {get; set;}</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>195</v>
-      </c>
-      <c r="B56" t="s">
-        <v>207</v>
-      </c>
-      <c r="C56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56" t="s">
-        <v>131</v>
-      </c>
-      <c r="F56" t="str">
-        <f t="shared" si="9"/>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>192</v>
+      </c>
+      <c r="B57" t="s">
+        <v>203</v>
+      </c>
+      <c r="C57" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="15"/>
         <v>public Guid ImageId {get; set;}</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
+      <c r="M57" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M58" t="s">
+        <v>243</v>
+      </c>
+      <c r="N58" t="s">
+        <v>159</v>
+      </c>
+      <c r="O58" t="s">
+        <v>112</v>
+      </c>
+      <c r="P58" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q58" t="str">
+        <f t="shared" ref="Q58:Q60" si="16">"public " &amp; O58 &amp; " "  &amp;  M58 &amp; " {get; set;}"</f>
+        <v>public Guid CategorySubCategoryMapId {get; set;}</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M59" t="s">
+        <v>237</v>
+      </c>
+      <c r="N59" t="s">
+        <v>159</v>
+      </c>
+      <c r="O59" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q59" t="str">
+        <f t="shared" si="16"/>
+        <v>public Guid CategoryId {get; set;}</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M60" t="s">
+        <v>199</v>
+      </c>
+      <c r="N60" t="s">
+        <v>159</v>
+      </c>
+      <c r="O60" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q60" t="str">
+        <f t="shared" si="16"/>
+        <v>public Guid SubCategoryId {get; set;}</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>226</v>
-      </c>
-      <c r="B65" t="s">
-        <v>227</v>
-      </c>
-      <c r="C65" t="s">
-        <v>113</v>
-      </c>
-      <c r="D65" t="s">
-        <v>131</v>
-      </c>
+      <c r="A65" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="B66" t="s">
+        <v>223</v>
+      </c>
+      <c r="C66" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66" t="s">
+        <v>130</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" ref="F66:F70" si="17">"public " &amp; C66 &amp; IF(D66="Y", "?","") &amp; " "  &amp;  A66 &amp; " {get; set;}"</f>
+        <v>public Guid AgentProductVariantPriceId {get; set;}</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>199</v>
+        <v>217</v>
+      </c>
+      <c r="B67" t="s">
+        <v>223</v>
+      </c>
+      <c r="C67" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="17"/>
+        <v>public Guid AgentId {get; set;}</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" t="s">
         <v>223</v>
       </c>
-      <c r="E68" t="s">
-        <v>224</v>
+      <c r="C68" t="s">
+        <v>112</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="17"/>
+        <v>public Guid ProductVariantId {get; set;}</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B73" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C69" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" t="s">
+        <v>220</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="17"/>
+        <v>public int PricingType {get; set;}</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>221</v>
+      </c>
+      <c r="B70" t="s">
+        <v>236</v>
+      </c>
+      <c r="C70" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" t="s">
+        <v>130</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="17"/>
+        <v>public decimal PricingValue {get; set;}</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>13</v>
-      </c>
-      <c r="B74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" t="s">
-        <v>113</v>
-      </c>
-      <c r="E74" t="s">
-        <v>4</v>
-      </c>
-      <c r="F74" t="str">
-        <f t="shared" ref="F74:F82" si="10">"public " &amp; C74 &amp; " "  &amp;  A74 &amp; " {get; set;}"</f>
-        <v>public Guid AddressID {get; set;}</v>
-      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B75" t="s">
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E75" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="10"/>
-        <v>public Guid UserID {get; set;}</v>
+        <f t="shared" ref="F75:F84" si="18">"public " &amp; C75 &amp; " "  &amp;  A75 &amp; " {get; set;}"</f>
+        <v>public Guid AddressID {get; set;}</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>15</v>
+        <v>264</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>197</v>
       </c>
       <c r="C76" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E76" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="10"/>
-        <v>public short AddressType {get; set;}</v>
+        <f t="shared" si="18"/>
+        <v>public Guid AddressMapId {get; set;}</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="C77" t="s">
-        <v>116</v>
+        <v>114</v>
+      </c>
+      <c r="E77" t="s">
+        <v>266</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="10"/>
-        <v>public string AddressLine1 {get; set;}</v>
+        <f t="shared" si="18"/>
+        <v>public short AddressType {get; set;}</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="10"/>
-        <v>public string AddressLine2 {get; set;}</v>
+        <f t="shared" si="18"/>
+        <v>public string AddressLine1 {get; set;}</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="10"/>
-        <v>public string City {get; set;}</v>
+        <f t="shared" si="18"/>
+        <v>public string AddressLine2 {get; set;}</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="10"/>
-        <v>public string PostCode {get; set;}</v>
+        <f t="shared" si="18"/>
+        <v>public string City {get; set;}</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C81" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="10"/>
-        <v>public string State {get; set;}</v>
+        <f t="shared" si="18"/>
+        <v>public string PostCode {get; set;}</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>115</v>
+      </c>
+      <c r="F82" t="str">
+        <f t="shared" si="18"/>
+        <v>public string State {get; set;}</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>22</v>
       </c>
-      <c r="B82" t="s">
-        <v>24</v>
-      </c>
-      <c r="C82" t="s">
-        <v>115</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="B83" t="s">
+        <v>197</v>
+      </c>
+      <c r="C83" t="s">
+        <v>112</v>
+      </c>
+      <c r="E83" t="s">
         <v>14</v>
       </c>
-      <c r="F82" t="str">
-        <f t="shared" si="10"/>
-        <v>public short CountryID {get; set;}</v>
+      <c r="F83" t="str">
+        <f t="shared" si="18"/>
+        <v>public Guid CountryID {get; set;}</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>267</v>
+      </c>
+      <c r="B84" t="s">
+        <v>151</v>
+      </c>
+      <c r="C84" t="s">
+        <v>160</v>
+      </c>
+      <c r="F84" t="str">
+        <f t="shared" si="18"/>
+        <v>public bool DefaultAddress {get; set;}</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" t="s">
+        <v>159</v>
+      </c>
+      <c r="C88" t="s">
+        <v>112</v>
+      </c>
+      <c r="D88" t="s">
+        <v>130</v>
+      </c>
+      <c r="E88" t="s">
+        <v>260</v>
+      </c>
+      <c r="F88" t="str">
+        <f t="shared" ref="F88:F92" si="19">"public " &amp; C88 &amp; " "  &amp;  A88 &amp; " {get; set;}"</f>
+        <v>public Guid AgentId {get; set;}</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>261</v>
+      </c>
+      <c r="B89" t="s">
+        <v>250</v>
+      </c>
+      <c r="C89" t="s">
+        <v>115</v>
+      </c>
+      <c r="D89" t="s">
+        <v>130</v>
+      </c>
+      <c r="F89" t="str">
+        <f t="shared" si="19"/>
+        <v>public string AgentName {get; set;}</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>262</v>
+      </c>
+      <c r="B90" t="s">
+        <v>59</v>
+      </c>
+      <c r="C90" t="s">
+        <v>115</v>
+      </c>
+      <c r="F90" t="str">
+        <f t="shared" si="19"/>
+        <v>public string AgentContactNo {get; set;}</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>263</v>
+      </c>
+      <c r="B91" t="s">
+        <v>215</v>
+      </c>
+      <c r="C91" t="s">
+        <v>115</v>
+      </c>
+      <c r="D91" t="s">
+        <v>130</v>
+      </c>
+      <c r="F91" t="str">
+        <f t="shared" si="19"/>
+        <v>public string AgentEmailId {get; set;}</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F92" t="str">
+        <f t="shared" si="19"/>
+        <v>public   {get; set;}</v>
       </c>
     </row>
     <row r="104" spans="7:17" x14ac:dyDescent="0.25">
@@ -2797,13 +3475,13 @@
         <v>24</v>
       </c>
       <c r="I107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K107" t="s">
         <v>4</v>
       </c>
       <c r="L107" t="str">
-        <f t="shared" ref="L107:L110" si="11">"public " &amp; I107 &amp; " "  &amp;  G107 &amp; " {get; set;}"</f>
+        <f t="shared" ref="L107:L110" si="20">"public " &amp; I107 &amp; " "  &amp;  G107 &amp; " {get; set;}"</f>
         <v>public short CurrencyID {get; set;}</v>
       </c>
       <c r="M107" t="s">
@@ -2813,10 +3491,10 @@
         <v>12</v>
       </c>
       <c r="O107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q107" t="str">
-        <f t="shared" ref="Q107:Q131" si="12">"public " &amp; O107 &amp; " "  &amp;  M107 &amp; " {get; set;}"</f>
+        <f t="shared" ref="Q107:Q131" si="21">"public " &amp; O107 &amp; " "  &amp;  M107 &amp; " {get; set;}"</f>
         <v>public short VoucherTypeID {get; set;}</v>
       </c>
     </row>
@@ -2828,10 +3506,10 @@
         <v>34</v>
       </c>
       <c r="I108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L108" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>public string CurrencyCode {get; set;}</v>
       </c>
       <c r="M108" t="s">
@@ -2841,10 +3519,10 @@
         <v>62</v>
       </c>
       <c r="O108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q108" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string VoucherType {get; set;}</v>
       </c>
     </row>
@@ -2856,10 +3534,10 @@
         <v>35</v>
       </c>
       <c r="I109" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L109" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>public string CurrencySymbol {get; set;}</v>
       </c>
       <c r="M109" t="s">
@@ -2869,10 +3547,10 @@
         <v>61</v>
       </c>
       <c r="O109" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q109" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string Description {get; set;}</v>
       </c>
     </row>
@@ -2884,10 +3562,10 @@
         <v>25</v>
       </c>
       <c r="I110" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L110" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>public string Currency {get; set;}</v>
       </c>
     </row>
@@ -2913,7 +3591,7 @@
     </row>
     <row r="114" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G114" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H114" s="5"/>
       <c r="I114" s="5"/>
@@ -2926,10 +3604,10 @@
         <v>3</v>
       </c>
       <c r="O114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q114" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public Guid AccountID {get; set;}</v>
       </c>
     </row>
@@ -2952,13 +3630,13 @@
         <v>3</v>
       </c>
       <c r="O115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P115" t="s">
         <v>14</v>
       </c>
       <c r="Q115" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public Guid UserID {get; set;}</v>
       </c>
     </row>
@@ -2970,13 +3648,13 @@
         <v>62</v>
       </c>
       <c r="O116" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P116" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q116" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string Account {get; set;}</v>
       </c>
     </row>
@@ -2988,10 +3666,10 @@
         <v>65</v>
       </c>
       <c r="O117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q117" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string CrDr {get; set;}</v>
       </c>
     </row>
@@ -3003,10 +3681,10 @@
         <v>61</v>
       </c>
       <c r="O118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q118" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string Description {get; set;}</v>
       </c>
     </row>
@@ -3018,10 +3696,10 @@
         <v>12</v>
       </c>
       <c r="O119" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q119" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public short ParentAccountID {get; set;}</v>
       </c>
     </row>
@@ -3037,19 +3715,19 @@
     </row>
     <row r="123" spans="7:17" x14ac:dyDescent="0.25">
       <c r="M123" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N123" t="s">
         <v>3</v>
       </c>
       <c r="O123" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P123" t="s">
         <v>4</v>
       </c>
       <c r="Q123" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public Guid AccountAddressID {get; set;}</v>
       </c>
     </row>
@@ -3061,13 +3739,13 @@
         <v>3</v>
       </c>
       <c r="O124" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P124" t="s">
         <v>14</v>
       </c>
       <c r="Q124" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public Guid AccountID {get; set;}</v>
       </c>
     </row>
@@ -3079,13 +3757,13 @@
         <v>12</v>
       </c>
       <c r="O125" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P125" t="s">
         <v>14</v>
       </c>
       <c r="Q125" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public short AddressType {get; set;}</v>
       </c>
     </row>
@@ -3097,10 +3775,10 @@
         <v>5</v>
       </c>
       <c r="O126" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q126" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string AddressLine1 {get; set;}</v>
       </c>
     </row>
@@ -3112,10 +3790,10 @@
         <v>5</v>
       </c>
       <c r="O127" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q127" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string AddressLine2 {get; set;}</v>
       </c>
     </row>
@@ -3127,10 +3805,10 @@
         <v>8</v>
       </c>
       <c r="O128" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q128" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string City {get; set;}</v>
       </c>
     </row>
@@ -3142,10 +3820,10 @@
         <v>23</v>
       </c>
       <c r="O129" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q129" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string PostCode {get; set;}</v>
       </c>
     </row>
@@ -3157,10 +3835,10 @@
         <v>8</v>
       </c>
       <c r="O130" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q130" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public string State {get; set;}</v>
       </c>
     </row>
@@ -3172,34 +3850,42 @@
         <v>24</v>
       </c>
       <c r="O131" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P131" t="s">
         <v>14</v>
       </c>
       <c r="Q131" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>public short CountryID {get; set;}</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="24">
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="G16:L16"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="G41:L41"/>
+    <mergeCell ref="G49:L49"/>
     <mergeCell ref="M122:P122"/>
     <mergeCell ref="G114:K114"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="M14:P14"/>
     <mergeCell ref="M105:P105"/>
     <mergeCell ref="M112:P112"/>
     <mergeCell ref="G106:K106"/>
-    <mergeCell ref="A73:E73"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="M37:R37"/>
+    <mergeCell ref="M45:R45"/>
+    <mergeCell ref="M51:R51"/>
+    <mergeCell ref="M57:R57"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="M14:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3287,7 +3973,7 @@
         <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>78</v>
@@ -3359,35 +4045,35 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
         <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3410,7 +4096,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1">
         <v>2010</v>
@@ -3418,7 +4104,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -3426,7 +4112,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3434,73 +4120,73 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3525,48 +4211,48 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="105" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>